<commit_message>
feat: proper formatting and parsing of link collection
</commit_message>
<xml_diff>
--- a/data/link_collection.xlsx
+++ b/data/link_collection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="127">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">author</t>
   </si>
   <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
     <t xml:space="preserve">keywords</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">2016-03-31</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=v1CmGbOGb2I</t>
+  </si>
+  <si>
     <t xml:space="preserve">functional programming, finance</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t xml:space="preserve">2021-10-26</t>
   </si>
   <si>
+    <t xml:space="preserve">https://fasterthanli.me/articles/my-ideal-rust-workflow</t>
+  </si>
+  <si>
     <t xml:space="preserve">rust</t>
   </si>
   <si>
@@ -79,6 +88,42 @@
     <t xml:space="preserve">blog</t>
   </si>
   <si>
+    <t xml:space="preserve">CS 253 Web Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-10-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stanford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/playlist?list=PL1y1iaEtjSYiiSGVlL1cHsXN_kvJOOhu-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web security, http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playlist for a full Stanford lecture on web security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 194 Introductio to Haskell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-01-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.seas.upenn.edu/~cis1940/spring13/lectures.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">functional programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture on Haskell and functional programming in general.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Machine Learning and Statistics</t>
   </si>
   <si>
@@ -91,10 +136,287 @@
     <t xml:space="preserve">Richard McElreath</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.youtube.com/playlist?list=PLDcUM9US4XdPz-KxHM4XHt7uUVGWWVSus</t>
+  </si>
+  <si>
     <t xml:space="preserve">bayesian statistics, statistical inference, scientific research</t>
   </si>
   <si>
     <t xml:space="preserve">Starts from the very principles and explains how we can reason about the world coming from a Bayesian point of view. Basically any content by Richard McElreath is of insanely high quality. Check out the Book “Statistical Rethinking” and accompanying code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science as Amateur Software Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-09-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=8qzVV7eEiaI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talk by Richard McElreath (highly recommended content in general) about the importance of software development in science.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stumpy docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://stumpy.readthedocs.io/en/latest/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time series analysis, machine learning, feature transformation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python library to compute matrix profile. Represent time series as nearest neighbor distance of a sliding window. Can be used to represent a time series and identify outliers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural Language Processing and LLMs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAG over complex PDFs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=oa82yoJ6zYc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural language processing, large language model, evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goes into detail how to set up a python app to perform retrieval augmented generation (RAG) over complex PDFs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive LLM Visualization in Browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brendan Bycroft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bbycroft.net/llm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insanely cool visualization of the dimensions of the matrices in a transformer model. Together with the tutorial videos by Karpathy really helps to create a good intution for the structure of LLMs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformer Slide Deck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucas Beyer (Google Deepmind)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lucasb.eyer.be/transformer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural language processing, large language model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice slide deck on the transformer logic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chunking Visualizer for RAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://chunkviz.up.railway.app/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">large language model, retrieval augmented generation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps to visualize different approaches for chunking that is relevant when building RAG apps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERTopic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maarten Grootendorst </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://maartengr.github.io/BERTopic/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">large language model, topic modeling, clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic mining library based on BERT and c-TF-IDF. Haven't used it myself but looks very promising.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perspectives on diffusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sander.ai/2023/07/20/perspectives.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diffusion models, midjourney, dalle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to diffusion models with a decent chunk of visualizations and sources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Diffusion: Building a Diffusion Model from linear Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-04-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.countbayesie.com/blog/2023/4/21/linear-diffusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explains the principles of a diffusion model and applies it to a linear approach to generate MNIST digits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance and Monetary System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zur Sinnhaftigkeit von Schuldenbremsen und Fiskalregeln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-20</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lars Feld </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(IFO Institute)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=EwxK5Rx7Kv4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debt management, interest rates, debt brake, fiscal deficits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This talk lays out the basic arguments for fiscal rules in general and specifically the debt brake in Germany. Since the topic is so frequently in media and talk shows, it is quite interesting to have the pro side of this debate laid out compactly. Aspect I would have liked a few words about: Focus on nominal debt vs interest expenses against background of recent low interest environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Money still matters for monetary policy presentation by Isabel Schnabel (ECB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-09-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabel Schnabel (ECB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ecb.europa.eu/press/key/date/2023/html/ecb.sp230925_1~7ad8ef22e2.en.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation, money supply, macroeconomics, monetary policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the recent decade of low inflation and nominal interest rates before covid, I thought it was quite interesting to read the view by the ECB on the inflation surge. Especially since it was argued in different outlets (talk shows, news papers, agencies) that the inflation was primarily a supply side shock, this analysis from the ECB seems quite balanced and acknowledges the potential inflationary pressure, depending on the regime a sovereign state is in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirk Ehnts über Staatsschulden &amp; die Modern Monetary Theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jung &amp; Naiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=wp1j11cmHbk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monetary policy, government deficit, modern monetary theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirk Ehnts is an advocate of modern monetary policy (MMT). In most cases I personally disagree with the assessments from advocates of the MMT school. However, I still find it interesting and valuable to follow the discussion and then come up with arguments as to why I disagree and would not recommend to follow the policy implications. Certainly the polar opposite to the lecture by Lars Feld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code based illustration of the Silicon Valley Bank Failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashwin Rao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://colab.research.google.com/drive/15uxrAeCCL327kWH9N0X-ogKwf2zErjP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bank failure, leverage, bond risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive and code based explanation of the Silicon Valley Bank failure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python google colab notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modern Monetary Theory – An Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bundestag.de/resource/blob/935936/4cb387b41e6fce9a1840f139a4c84b29/WD-4-113-22-pdf-data.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report from the German Bundestag that lays our major points of criticism regarding the practical application of Modern Monetary Theory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual Reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture on virtual or digitized Humans at MPI Tübingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/playlist?list=PL05umP7R6ij13it8Rptqo7lycHozvzCJn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virtual reality, machine learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since I am a big fan of virtual reality, the concepts of trying to digitize humans is very interesting to me. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesswrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lesswrong.com/rationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cognitive biases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popular blog dedicated to learning about cognitive biases and improving rational reasoning.</t>
   </si>
 </sst>
 </file>
@@ -106,7 +428,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -127,6 +449,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +498,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,6 +520,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,17 +654,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,88 +684,577 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>45659</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>45659</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="I4" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="98.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>45659</v>
+      <c r="I14" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="131.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="153.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>44953</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="5" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="5" t="n">
+        <v>45445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add more links
</commit_message>
<xml_diff>
--- a/data/link_collection.xlsx
+++ b/data/link_collection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="154">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -124,6 +124,39 @@
     <t xml:space="preserve">Lecture on Haskell and functional programming in general.</t>
   </si>
   <si>
+    <t xml:space="preserve">Zig and Rust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex Kladov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://matklad.github.io/2023/03/26/zig-and-rust.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rust, zig, programming languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This post compares Rust and Zig, which are quite popular at the moment, in terms of design and tooling. But this blog has in general many insightful articles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mediocre Engineer’s guide to HTTPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devon Peroutky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://devonperoutky.super.site/blog-posts/mediocre-engineers-guide-to-https</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http, web development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides some nice visualizations on the http lifecycle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Machine Learning and Statistics</t>
   </si>
   <si>
@@ -283,6 +316,54 @@
     <t xml:space="preserve">Explains the principles of a diffusion model and applies it to a linear approach to generate MNIST digits.</t>
   </si>
   <si>
+    <t xml:space="preserve">How diffusion models work: the math from scratch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-09-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sergios Karagiannakos, Nikolas Adaloglou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://theaisummer.com/diffusion-models/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diffusion models, math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkthrough of math in diffusion models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defusing Diffusion Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-02-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paweł A. Pierzchlewicz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://perceptron.blog/defusing-diffusion/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to diffusion model maths with very nice visualizations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Annotated Diffusion Model </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-06-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niels Rogge, Kashif Rasul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diffusion models, pytorch, python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial for diffusion models with extensive code samples in pytorch</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finance and Monetary System</t>
   </si>
   <si>
@@ -292,23 +373,7 @@
     <t xml:space="preserve">2023-11-20</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lars Feld </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(IFO Institute)</t>
-    </r>
+    <t xml:space="preserve">Lars Feld (IFO Institute)</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.youtube.com/watch?v=EwxK5Rx7Kv4</t>
@@ -428,7 +493,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -449,11 +514,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -498,12 +558,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,24 +571,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -654,17 +710,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.14"/>
   </cols>
   <sheetData>
@@ -672,36 +728,36 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -711,24 +767,24 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="4" t="n">
         <v>45445</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -738,522 +794,663 @@
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="4" t="n">
         <v>45445</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="4" t="n">
         <v>45445</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="I5" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="98.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="I8" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="I9" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="I11" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="5" t="n">
+      <c r="H12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="4" t="n">
         <v>45445</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="0" t="s">
+      <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="I14" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="131.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="I16" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="153.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="H17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="D18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="I18" s="4" t="n">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="0" t="s">
+      <c r="G19" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="131.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="I19" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="5" t="n">
+      <c r="I21" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="153.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="77.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="4" t="n">
         <v>44953</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="0" t="s">
+      <c r="E25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="5" t="n">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" s="0" t="s">
+      <c r="I26" s="4" t="n">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="5" t="n">
+      <c r="I27" s="4" t="n">
         <v>45445</v>
       </c>
     </row>

</xml_diff>